<commit_message>
Updated DBer details and change password feature added
</commit_message>
<xml_diff>
--- a/DBPortal/media/excel_sheets/Testing.xlsx
+++ b/DBPortal/media/excel_sheets/Testing.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">aadhar</t>
   </si>
   <si>
-    <t xml:space="preserve">first</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last</t>
+    <t xml:space="preserve">Full Name</t>
   </si>
   <si>
     <t xml:space="preserve">dob</t>
@@ -43,16 +40,13 @@
     <t xml:space="preserve">city</t>
   </si>
   <si>
-    <t xml:space="preserve">ayush</t>
-  </si>
-  <si>
-    <t xml:space="preserve">agrawal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Punjab</t>
+    <t xml:space="preserve">jhjh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajasthan</t>
   </si>
   <si>
     <t xml:space="preserve">Patiala</t>
@@ -157,19 +151,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -191,31 +184,25 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>123456789012</v>
+        <v>111111111111</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>37336</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>36901</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>